<commit_message>
Added practice feedback, randomization of items.
</commit_message>
<xml_diff>
--- a/data_raw/dicts/SRS_dict.xlsx
+++ b/data_raw/dicts/SRS_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B53E08-44F6-4E33-A22F-491CC7C89D52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C4E836-A899-40B6-A0BB-FB0075606978}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>key</t>
   </si>
@@ -37,119 +37,137 @@
     <t>INSTRUCTIONS</t>
   </si>
   <si>
-    <t>You will now read several series of words or short phrases. In some of these series, one element has a different rhythm from the others. &lt;br/&gt; Your task is to judge whether the row contains a rhythmically unsuitable element and, if so, to mark the corresponding element. To do this, simply click on the corresponding word.</t>
-  </si>
-  <si>
-    <t>Sie werden nun mehrere Reihen von Wörtern bzw. kurzen Phrasen lesen. In einigen dieser Reihen weist jeweils ein Element einen anderen Rhythmus auf als die übrigen. &lt;br/&gt;
+    <t>PROMPT</t>
+  </si>
+  <si>
+    <t>ALL_EQUAL</t>
+  </si>
+  <si>
+    <t>Alle gleich</t>
+  </si>
+  <si>
+    <t>All equal</t>
+  </si>
+  <si>
+    <t>SRS_FEEDBACK</t>
+  </si>
+  <si>
+    <t>EXAMPLE_HEADER</t>
+  </si>
+  <si>
+    <t>PAGE_COUNTER</t>
+  </si>
+  <si>
+    <t>Seite {{page_no}} von {{num_pages}}</t>
+  </si>
+  <si>
+    <t>Page {{page_no}} of {{num_pages}}</t>
+  </si>
+  <si>
+    <t>WELCOME</t>
+  </si>
+  <si>
+    <t>Test zur Rhythmuswahrnehmung in Sprache</t>
+  </si>
+  <si>
+    <t>Welcome to the Speech Rhythm Sensitivity Test!</t>
+  </si>
+  <si>
+    <t>Willkommen zum Test für Rhythmuswahrnehmung in der Sprache!</t>
+  </si>
+  <si>
+    <t>PRACTICE_ITEMS</t>
+  </si>
+  <si>
+    <t>Düse,Trommel,Erde,Besteck</t>
+  </si>
+  <si>
+    <t>PRACTICE_ITEMS_EMPH</t>
+  </si>
+  <si>
+    <t>DÜse,TROMmel,ERde,BeSTECK</t>
+  </si>
+  <si>
+    <t>CONTINUE_MAIN_TEST</t>
+  </si>
+  <si>
+    <t>Nun geht der Test los.&lt;br&gt; Viel Vergnügen!</t>
+  </si>
+  <si>
+    <t>Now the test starts.&lt;br&gt; Have fun!</t>
+  </si>
+  <si>
+    <t>Beispiel {{page_no}} von {{num_pages}}</t>
+  </si>
+  <si>
+    <t>Example {{page_no}} of {{num_pages}}</t>
+  </si>
+  <si>
+    <t>EXAMPLE</t>
+  </si>
+  <si>
+    <t>EXAMPLE_PROMPT</t>
+  </si>
+  <si>
+    <t>Hier zunächst ein Beispiel.</t>
+  </si>
+  <si>
+    <t>First, an example.</t>
+  </si>
+  <si>
+    <t>A Sample Question</t>
+  </si>
+  <si>
+    <t>Eine Beispielaufgabe</t>
+  </si>
+  <si>
+    <t>Sie haben {{num_correct}} von {{num_items}} Fragen richtig beantwortet ({{perc_correct}}%).</t>
+  </si>
+  <si>
+    <t>You answered {{num_correct}} out of {{num_items}} questions correct ({{perc_correct}}%).</t>
+  </si>
+  <si>
+    <t>Ist der Rhythmus aller Wörter gleich oder ist eins unpassend? &lt;br/&gt; Klicken Sie auf das Wort, das herausfällt oder wählen Sie "Alle gleich". &lt;br/&gt; Sie haben {{time_out}} Sekunden Zeit zu antworten.</t>
+  </si>
+  <si>
+    <t>Is the rhythm of all words equal or does one not fit to the others? Click on the word, that does not fit or on "All equal". &lt;br/&gt;You got {{time_out}} seconds to answer.</t>
+  </si>
+  <si>
+    <t>SRS_TESTNAME</t>
+  </si>
+  <si>
+    <t>Sie werden nun mehrere Reihen von Wörtern bzw. kurzen Phrasen lesen. In einigen dieser Reihen weist jeweils ein Element einen anderen Rhythmus auf als die übrigen. Achten Sie deshalb besonders auf die Betonungen und Akzente der Wörter.&lt;br/&gt;
 Ihre Aufgabe besteht darin, zu beurteilen, ob die Reihe ein rhythmisch unpassendes Element enthält und ggf. das entsprechende Element zu markieren. Klicken Sie dazu einfach auf das entsprechende Wort</t>
   </si>
   <si>
-    <t>PROMPT</t>
-  </si>
-  <si>
-    <t>ALL_EQUAL</t>
-  </si>
-  <si>
-    <t>Alle gleich</t>
-  </si>
-  <si>
-    <t>All equal</t>
-  </si>
-  <si>
-    <t>SRS_FEEDBACK</t>
-  </si>
-  <si>
-    <t>EXAMPLE_HEADER</t>
-  </si>
-  <si>
-    <t>PAGE_COUNTER</t>
-  </si>
-  <si>
-    <t>Seite {{page_no}} von {{num_pages}}</t>
-  </si>
-  <si>
-    <t>Page {{page_no}} of {{num_pages}}</t>
-  </si>
-  <si>
-    <t>WELCOME</t>
-  </si>
-  <si>
-    <t>Test zur Rhythmuswahrnehmung in Sprache</t>
-  </si>
-  <si>
-    <t>Welcome to the Speech Rhythm Sensitivity Test!</t>
-  </si>
-  <si>
-    <t>Willkommen zum Test für Rhythmuswahrnehmung in der Sprache!</t>
-  </si>
-  <si>
-    <t>PRACTICE_ITEMS</t>
-  </si>
-  <si>
-    <t>Düse,Trommel,Erde,Besteck</t>
-  </si>
-  <si>
-    <t>PRACTICE_ITEMS_EMPH</t>
-  </si>
-  <si>
-    <t>DÜse,TROMmel,ERde,BeSTECK</t>
-  </si>
-  <si>
-    <t>CONTINUE_MAIN_TEST</t>
-  </si>
-  <si>
-    <t>Nun geht der Test los.&lt;br&gt; Viel Vergnügen!</t>
-  </si>
-  <si>
-    <t>Now the test starts.&lt;br&gt; Have fun!</t>
-  </si>
-  <si>
-    <t>Beispiel {{page_no}} von {{num_pages}}</t>
-  </si>
-  <si>
-    <t>Example {{page_no}} of {{num_pages}}</t>
-  </si>
-  <si>
-    <t>EXAMPLE</t>
-  </si>
-  <si>
-    <t>EXAMPLE_PROMPT</t>
-  </si>
-  <si>
-    <t>Hier zunächst ein Beispiel.</t>
-  </si>
-  <si>
-    <t>First, an example.</t>
-  </si>
-  <si>
-    <t>EXAMPLE_FEEDBACK</t>
-  </si>
-  <si>
-    <t>Correct, BeSTECK did not fit rhythmically.</t>
-  </si>
-  <si>
-    <t>A Sample Question</t>
-  </si>
-  <si>
-    <t>Eine Beispielaufgabe</t>
-  </si>
-  <si>
-    <t>Sie haben {{num_correct}} von {{num_items}} Fragen richtig beantwortet ({{perc_correct}}%).</t>
-  </si>
-  <si>
-    <t>You answered {{num_correct}} out of {{num_items}} questions correct ({{perc_correct}}%).</t>
-  </si>
-  <si>
-    <t>Ist der Rhythmus aller Wörter gleich oder ist eins unpassend? &lt;br/&gt; Klicken Sie auf das Wort, das herausfällt oder wählen Sie "Alle gleich". &lt;br/&gt; Sie haben {{time_out}} Sekunden Zeit zu antworten.</t>
-  </si>
-  <si>
-    <t>Is the rhythm of all words equal or does one not fit to the others? Click on the word, that does not fit or on "All equal". &lt;br/&gt;You got {{time_out}} seconds to answer.</t>
-  </si>
-  <si>
-    <t>SRS_TESTNAME</t>
-  </si>
-  <si>
-    <t>Korrekt, BeSTECK ist rhythmisch unpassend.</t>
+    <t>You will now read several series of words or short phrases. In some of these series, one element has a different rhythm from the others. Therefore, pay special attention to the stresses and accents of the words.&lt;br/&gt; Your task is to judge whether the row contains a rhythmically unsuitable element and, if so, to mark the corresponding element. To do this, simply click on the corresponding word.</t>
+  </si>
+  <si>
+    <t>EXAMPLE_FEEDBACK_CORRECT</t>
+  </si>
+  <si>
+    <t>The answer was not correct. Please try again!</t>
+  </si>
+  <si>
+    <t>Das war leider nicht richtig. Versuchen Sie es nochmal!</t>
+  </si>
+  <si>
+    <t>Das war leider zu langsam. Versuchen Sie es nochmal!</t>
+  </si>
+  <si>
+    <t>This was too slow. Please try again!</t>
+  </si>
+  <si>
+    <t>EXAMPLE_FEEDBACK_TOO_SLOW</t>
+  </si>
+  <si>
+    <t>EXAMPLE_FEEDBACK_INCORRECT</t>
+  </si>
+  <si>
+    <t>Korrekt, ReVIER ist rhythmisch unpassend.</t>
+  </si>
+  <si>
+    <t>Correct, ReVIER did not fit rhythmically.</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,10 +1039,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1035,142 +1053,164 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
-        <v>34</v>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added first version of ART (Artist Recognition Test)
</commit_message>
<xml_diff>
--- a/data_raw/dicts/SRS_dict.xlsx
+++ b/data_raw/dicts/SRS_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C4E836-A899-40B6-A0BB-FB0075606978}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0230F4D4-2530-4D35-90E7-4664C7730571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>key</t>
   </si>
@@ -49,9 +49,6 @@
     <t>All equal</t>
   </si>
   <si>
-    <t>SRS_FEEDBACK</t>
-  </si>
-  <si>
     <t>EXAMPLE_HEADER</t>
   </si>
   <si>
@@ -88,15 +85,6 @@
     <t>DÜse,TROMmel,ERde,BeSTECK</t>
   </si>
   <si>
-    <t>CONTINUE_MAIN_TEST</t>
-  </si>
-  <si>
-    <t>Nun geht der Test los.&lt;br&gt; Viel Vergnügen!</t>
-  </si>
-  <si>
-    <t>Now the test starts.&lt;br&gt; Have fun!</t>
-  </si>
-  <si>
     <t>Beispiel {{page_no}} von {{num_pages}}</t>
   </si>
   <si>
@@ -131,9 +119,6 @@
   </si>
   <si>
     <t>Is the rhythm of all words equal or does one not fit to the others? Click on the word, that does not fit or on "All equal". &lt;br/&gt;You got {{time_out}} seconds to answer.</t>
-  </si>
-  <si>
-    <t>SRS_TESTNAME</t>
   </si>
   <si>
     <t>Sie werden nun mehrere Reihen von Wörtern bzw. kurzen Phrasen lesen. In einigen dieser Reihen weist jeweils ein Element einen anderen Rhythmus auf als die übrigen. Achten Sie deshalb besonders auf die Betonungen und Akzente der Wörter.&lt;br/&gt;
@@ -168,6 +153,12 @@
   </si>
   <si>
     <t>Correct, ReVIER did not fit rhythmically.</t>
+  </si>
+  <si>
+    <t>TESTNAME</t>
+  </si>
+  <si>
+    <t>FEEDBACK</t>
   </si>
 </sst>
 </file>
@@ -1014,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,10 +1030,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1053,10 +1044,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,10 +1055,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1083,134 +1074,123 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>24</v>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added second sample item to SRS, shortened item prompt.
</commit_message>
<xml_diff>
--- a/data_raw/dicts/SRS_dict.xlsx
+++ b/data_raw/dicts/SRS_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44A6F35-C4C4-450C-B900-CA3435747873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3626F9FB-AA74-4C01-ACAF-5C96F5F3AD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>key</t>
   </si>
@@ -85,24 +85,12 @@
     <t>Example {{page_no}} of {{num_pages}}</t>
   </si>
   <si>
-    <t>EXAMPLE</t>
-  </si>
-  <si>
-    <t>EXAMPLE_PROMPT</t>
-  </si>
-  <si>
     <t>Hier zunächst ein Beispiel.</t>
   </si>
   <si>
     <t>First, an example.</t>
   </si>
   <si>
-    <t>A Sample Question</t>
-  </si>
-  <si>
-    <t>Eine Beispielaufgabe</t>
-  </si>
-  <si>
     <t>Sie haben {{num_correct}} von {{num_items}} Fragen richtig beantwortet ({{perc_correct}}%).</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
   </si>
   <si>
     <t>Is the rhythm of all words equal or does one not fit to the others? Click on the word, that does not fit or on "All equal". &lt;br/&gt;You got {{time_out}} seconds to answer.</t>
-  </si>
-  <si>
-    <t>EXAMPLE_FEEDBACK_CORRECT</t>
   </si>
   <si>
     <t>The answer was not correct. Please try again!</t>
@@ -159,6 +144,58 @@
   </si>
   <si>
     <t>We will now present you with some series of four individual words or short expressions each, e.g. plate - box - rat - parquet.  Please read these series carefully, paying particular  attention to the rhythm of speech, i.e. the stress patterns of the words. &lt;br/&gt; In some of these series, however, there is exactly one element that has a different stress pattern than the others - in the example above it is the word "parquet".  Your task is to judge for each row whether or not there is an element with a different stress pattern.  If all the elements in the row have the same stress pattern, please click on the field "All equal".  If an element has a different stress pattern, please click on the field of this different element. &lt;br/&gt;Please note that you have **{{time_out}} seconds** for each row to make your judgement.</t>
+  </si>
+  <si>
+    <t>EXAMPLE_FEEDBACK_CORRECT1</t>
+  </si>
+  <si>
+    <t>EXAMPLE_FEEDBACK_CORRECT2</t>
+  </si>
+  <si>
+    <t>Korrekt, alle hatten dasselbe Betonungsmuster.</t>
+  </si>
+  <si>
+    <t>Correct, all had the same rhythm.</t>
+  </si>
+  <si>
+    <t>EXAMPLE2</t>
+  </si>
+  <si>
+    <t>Zweite Beispielaufgabe</t>
+  </si>
+  <si>
+    <t>Second Sample Question</t>
+  </si>
+  <si>
+    <t>EXAMPLE1</t>
+  </si>
+  <si>
+    <t>Erste Beispielaufgabe</t>
+  </si>
+  <si>
+    <t>First Sample Question</t>
+  </si>
+  <si>
+    <t>EXAMPLE_PROMPT2</t>
+  </si>
+  <si>
+    <t>Hier noch ein Beispiel.</t>
+  </si>
+  <si>
+    <t>Another example.</t>
+  </si>
+  <si>
+    <t>EXAMPLE_PROMPT1</t>
+  </si>
+  <si>
+    <t>PROMPT_SHORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ist der Rhythmus aller Wörter gleich oder hat eines ein abweichendes Betonungsmuster?
+</t>
+  </si>
+  <si>
+    <t>Is the rhythm of all words equal or does one not fit to the others?</t>
   </si>
 </sst>
 </file>
@@ -1002,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,10 +1065,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -1042,10 +1079,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -1053,10 +1090,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -1073,13 +1110,13 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1109,7 +1146,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -1139,57 +1176,101 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>